<commit_message>
matricula IMAMUN y ARMUN
</commit_message>
<xml_diff>
--- a/matri/an.xlsx
+++ b/matri/an.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Colegío\M.U.N\MAPISMUN\mapismun_pag\matri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5C001D-F2B3-49AB-BDDD-7F554909C09D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57277D2B-7207-4491-AF29-786AF5EED28B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -460,6 +460,105 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -472,109 +571,16 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -941,21 +947,21 @@
   <dimension ref="A6:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:E26"/>
+      <selection activeCell="D27" sqref="D27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="8"/>
       <c r="G6" s="1"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -964,48 +970,48 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="G8" s="39" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="G8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1014,36 +1020,36 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="G10" s="29" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="G11" s="19" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="G11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="21"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
@@ -1056,183 +1062,183 @@
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="G13" s="19" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="G13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="44"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
       <c r="F26" s="4"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="46"/>
       <c r="F27" s="4"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="4"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="4"/>
       <c r="G29" s="1"/>
     </row>
@@ -1249,6 +1255,50 @@
     <sortCondition ref="A22"/>
   </sortState>
   <mergeCells count="51">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:J10"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="A7:E7"/>
@@ -1256,50 +1306,6 @@
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="G8:K8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>